<commit_message>
tentar arranjar problemas de dimensao
</commit_message>
<xml_diff>
--- a/apa/Fmedia2017.xlsx
+++ b/apa/Fmedia2017.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,9 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -425,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH6"/>
+  <dimension ref="A1:BI6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,1035 +442,1055 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Alverca</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Anta-Espinho</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Arcos</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Aveiro</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Avenida da Liberdade</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Avintes</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Burgães-Santo Tirso</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Cascais - Escola da Cidadela</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Cerro</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Chamusca</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Cónego Dr. Manuel Faria-Azurém</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>David Neto</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>D.Manuel II-Vermoim</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Douro Norte</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Entrecampos</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Ermesinde-Valongo</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Escavadeira</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Estarreja/ Teixugueira</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Faial</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Fernando Pó</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Fidalguinhos</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Fornelo do Monte</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Francisco Sá Carneiro-Campanha</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Fr Bartolomeu Mártires-S.Vitor</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Frossos-Braga</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Fundão</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Ílhavo</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Instituto Geofísico de Coimbra</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>João Gomes Laranjo-S.Hora</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>Joaquim Magalhães</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>Laranjeiro</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>Lavradio</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>Leça do Balio-Matosinhos</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Loures-Centro</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>Lourinhã</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Malpique</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>Meco-Perafita</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>Mem Martins</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>Mindelo-Vila do Conde</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>Monte Chãos</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Montemor-o-Velho</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Monte Velho</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>Odivelas-Ramada</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>Olivais</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Paços de Ferreira</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Paio Pires</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Pe Moreira Neves-Castelões de Cepeda</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>Quebedo</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Quinta do Marquês</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Reboleira</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Santa Cruz de Benfica</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>Santana</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>Santiago do Cacém</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>São Gonçalo</t>
         </is>
       </c>
-      <c r="BC1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>São João</t>
         </is>
       </c>
-      <c r="BD1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>Seara-Matosinhos</t>
         </is>
       </c>
-      <c r="BE1" s="1" t="inlineStr">
+      <c r="BF1" s="1" t="inlineStr">
         <is>
           <t>Sonega</t>
         </is>
       </c>
-      <c r="BF1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>Terena</t>
         </is>
       </c>
-      <c r="BG1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>VNTelha-Maia</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>proporção</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="2" t="n">
+        <v>43022</v>
+      </c>
+      <c r="B2" t="n">
         <v>54.3</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>42.20833333333334</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>54.0625</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>44.79166666666666</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>61.9625</v>
       </c>
-      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="n">
         <v>53.90416666666667</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>32.04166666666666</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>36.03333333333333</v>
       </c>
-      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="n">
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="n">
         <v>49.99583333333334</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>46.33333333333334</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>3.939130434782609</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>58.69583333333333</v>
       </c>
-      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
-      <c r="X2" t="n">
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="n">
         <v>29.04761904761905</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="Z2" t="n">
         <v>13.41666666666667</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AA2" t="n">
         <v>35</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AB2" t="n">
         <v>33.33333333333334</v>
       </c>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="n">
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="n">
         <v>48.08333333333334</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AE2" t="n">
         <v>32.04583333333333</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AF2" t="n">
         <v>42.85416666666666</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AG2" t="n">
         <v>46.6</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AH2" t="n">
         <v>13.20833333333333</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AI2" t="n">
         <v>38.3625</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AJ2" t="n">
         <v>37.65416666666666</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AK2" t="n">
         <v>45.15416666666667</v>
       </c>
-      <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="n">
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="n">
         <v>35.025</v>
       </c>
-      <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="inlineStr"/>
-      <c r="AO2" t="n">
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="n">
         <v>37.83333333333334</v>
       </c>
-      <c r="AP2" t="n">
+      <c r="AQ2" t="n">
         <v>59.41666666666666</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="AR2" t="n">
         <v>54.24583333333334</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AS2" t="n">
         <v>51.61666666666667</v>
       </c>
-      <c r="AS2" t="inlineStr"/>
-      <c r="AT2" t="n">
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="n">
         <v>62.26666666666667</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="AV2" t="n">
         <v>18.95833333333333</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="AW2" t="n">
         <v>61.11666666666667</v>
       </c>
-      <c r="AW2" t="n">
+      <c r="AX2" t="n">
         <v>38.85833333333333</v>
       </c>
-      <c r="AX2" t="n">
+      <c r="AY2" t="n">
         <v>48.65416666666667</v>
       </c>
-      <c r="AY2" t="n">
+      <c r="AZ2" t="n">
         <v>71.80833333333334</v>
       </c>
-      <c r="AZ2" t="n">
+      <c r="BA2" t="n">
         <v>51.04583333333333</v>
       </c>
-      <c r="BA2" t="n">
+      <c r="BB2" t="n">
         <v>36.91666666666666</v>
       </c>
-      <c r="BB2" t="n">
+      <c r="BC2" t="n">
         <v>56.93333333333334</v>
       </c>
-      <c r="BC2" t="n">
+      <c r="BD2" t="n">
         <v>79.25833333333334</v>
       </c>
-      <c r="BD2" t="n">
+      <c r="BE2" t="n">
         <v>40.5</v>
       </c>
-      <c r="BE2" t="n">
+      <c r="BF2" t="n">
         <v>33.08333333333334</v>
       </c>
-      <c r="BF2" t="n">
+      <c r="BG2" t="n">
         <v>55.08333333333334</v>
       </c>
-      <c r="BG2" t="n">
+      <c r="BH2" t="n">
         <v>47.83333333333334</v>
       </c>
-      <c r="BH2" t="n">
-        <v>0.7288135593220338</v>
+      <c r="BI2" t="n">
+        <v>0.7333333333333333</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="2" t="n">
+        <v>43023</v>
+      </c>
+      <c r="B3" t="n">
         <v>59.06666666666666</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>63.33333333333334</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>49.92916666666667</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>73.45833333333333</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>57.40833333333333</v>
       </c>
-      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="n">
         <v>30.84166666666667</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>47.19583333333333</v>
       </c>
-      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="n">
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="n">
         <v>59.05</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>72.54166666666667</v>
       </c>
-      <c r="S3" t="n">
+      <c r="T3" t="n">
         <v>8.4125</v>
       </c>
-      <c r="T3" t="n">
+      <c r="U3" t="n">
         <v>61.17083333333333</v>
       </c>
-      <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="n">
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="n">
         <v>5.857142857142857</v>
       </c>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="n">
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="n">
         <v>51.41666666666666</v>
       </c>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="n">
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="n">
         <v>64.66666666666667</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AE3" t="n">
         <v>33.6625</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AF3" t="n">
         <v>50.14583333333334</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="AG3" t="n">
         <v>48.56315789473685</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="AH3" t="n">
         <v>16.625</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="AI3" t="n">
         <v>44.09166666666667</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="AJ3" t="n">
         <v>62.04166666666666</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="AK3" t="n">
         <v>51.2</v>
       </c>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="n">
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="n">
         <v>42.5375</v>
       </c>
-      <c r="AM3" t="inlineStr"/>
       <c r="AN3" t="inlineStr"/>
-      <c r="AO3" t="n">
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="n">
         <v>82.125</v>
       </c>
-      <c r="AP3" t="n">
+      <c r="AQ3" t="n">
         <v>51.08333333333334</v>
       </c>
-      <c r="AQ3" t="n">
+      <c r="AR3" t="n">
         <v>62.61666666666667</v>
       </c>
-      <c r="AR3" t="n">
+      <c r="AS3" t="n">
         <v>56.67083333333333</v>
       </c>
-      <c r="AS3" t="inlineStr"/>
-      <c r="AT3" t="n">
+      <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="n">
         <v>67.27083333333333</v>
       </c>
-      <c r="AU3" t="n">
+      <c r="AV3" t="n">
         <v>22.70833333333333</v>
       </c>
-      <c r="AV3" t="n">
+      <c r="AW3" t="n">
         <v>58.8375</v>
       </c>
-      <c r="AW3" t="n">
+      <c r="AX3" t="n">
         <v>42.34583333333333</v>
       </c>
-      <c r="AX3" t="n">
+      <c r="AY3" t="n">
         <v>50.81666666666666</v>
       </c>
-      <c r="AY3" t="n">
+      <c r="AZ3" t="n">
         <v>61.80869565217391</v>
       </c>
-      <c r="AZ3" t="n">
+      <c r="BA3" t="n">
         <v>52.725</v>
       </c>
-      <c r="BA3" t="n">
+      <c r="BB3" t="n">
         <v>39.25</v>
       </c>
-      <c r="BB3" t="n">
+      <c r="BC3" t="n">
         <v>54.88333333333333</v>
       </c>
-      <c r="BC3" t="n">
+      <c r="BD3" t="n">
         <v>59.99166666666667</v>
       </c>
-      <c r="BD3" t="n">
+      <c r="BE3" t="n">
         <v>56.5</v>
       </c>
-      <c r="BE3" t="n">
+      <c r="BF3" t="n">
         <v>31.25</v>
       </c>
-      <c r="BF3" t="n">
+      <c r="BG3" t="n">
         <v>58.375</v>
       </c>
-      <c r="BG3" t="n">
+      <c r="BH3" t="n">
         <v>59.29166666666666</v>
       </c>
-      <c r="BH3" t="n">
-        <v>0.6779661016949152</v>
+      <c r="BI3" t="n">
+        <v>0.6833333333333333</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="2" t="n">
+        <v>43024</v>
+      </c>
+      <c r="B4" t="n">
         <v>64.25833333333334</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>54.5</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>64.60000000000001</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>93</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>67.82083333333334</v>
       </c>
-      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
-      <c r="J4" t="n">
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="n">
         <v>82.32916666666667</v>
       </c>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="n">
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="n">
         <v>15.6375</v>
       </c>
-      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="n">
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="n">
         <v>57.35238095238095</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>75.95833333333333</v>
       </c>
-      <c r="S4" t="n">
+      <c r="T4" t="n">
         <v>6.733333333333333</v>
       </c>
-      <c r="T4" t="n">
+      <c r="U4" t="n">
         <v>59.12916666666667</v>
       </c>
-      <c r="U4" t="n">
+      <c r="V4" t="n">
         <v>64.29473684210525</v>
       </c>
-      <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
       <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="n">
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="n">
         <v>42.125</v>
       </c>
-      <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="n">
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="n">
         <v>61.125</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AE4" t="n">
         <v>62.42083333333333</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AF4" t="n">
         <v>70.88333333333334</v>
       </c>
-      <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="n">
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="n">
         <v>15</v>
       </c>
-      <c r="AH4" t="n">
+      <c r="AI4" t="n">
         <v>58.82083333333333</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="AJ4" t="n">
         <v>55.49166666666667</v>
       </c>
-      <c r="AJ4" t="n">
+      <c r="AK4" t="n">
         <v>93.83749999999999</v>
       </c>
-      <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="n">
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="n">
         <v>65.85000000000001</v>
       </c>
-      <c r="AM4" t="inlineStr"/>
       <c r="AN4" t="inlineStr"/>
-      <c r="AO4" t="n">
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="n">
         <v>196.4166666666667</v>
       </c>
-      <c r="AP4" t="n">
+      <c r="AQ4" t="n">
         <v>78.05</v>
       </c>
-      <c r="AQ4" t="n">
+      <c r="AR4" t="n">
         <v>67.63333333333334</v>
       </c>
-      <c r="AR4" t="n">
+      <c r="AS4" t="n">
         <v>55.49583333333334</v>
       </c>
-      <c r="AS4" t="n">
+      <c r="AT4" t="n">
         <v>119.2916666666667</v>
       </c>
-      <c r="AT4" t="n">
+      <c r="AU4" t="n">
         <v>63.975</v>
       </c>
-      <c r="AU4" t="n">
+      <c r="AV4" t="n">
         <v>48.04166666666666</v>
       </c>
-      <c r="AV4" t="n">
+      <c r="AW4" t="n">
         <v>57.2</v>
       </c>
-      <c r="AW4" t="n">
+      <c r="AX4" t="n">
         <v>57.35</v>
       </c>
-      <c r="AX4" t="n">
+      <c r="AY4" t="n">
         <v>49.3375</v>
       </c>
-      <c r="AY4" t="inlineStr"/>
-      <c r="AZ4" t="n">
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="n">
         <v>9.433333333333334</v>
       </c>
-      <c r="BA4" t="n">
+      <c r="BB4" t="n">
         <v>82.69565217391305</v>
       </c>
-      <c r="BB4" t="n">
+      <c r="BC4" t="n">
         <v>9.970833333333333</v>
       </c>
-      <c r="BC4" t="n">
+      <c r="BD4" t="n">
         <v>15.28333333333333</v>
       </c>
-      <c r="BD4" t="n">
+      <c r="BE4" t="n">
         <v>55.66666666666666</v>
       </c>
-      <c r="BE4" t="n">
+      <c r="BF4" t="n">
         <v>34.91666666666666</v>
       </c>
-      <c r="BF4" t="n">
+      <c r="BG4" t="n">
         <v>59.20833333333334</v>
       </c>
-      <c r="BG4" t="inlineStr"/>
-      <c r="BH4" t="n">
-        <v>0.6440677966101694</v>
+      <c r="BH4" t="inlineStr"/>
+      <c r="BI4" t="n">
+        <v>0.65</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="2" t="n">
+        <v>43025</v>
+      </c>
+      <c r="B5" t="n">
         <v>28.80833333333333</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>17.54166666666667</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>31.15833333333333</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>45</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>23.59166666666667</v>
       </c>
-      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="n">
         <v>19.09473684210526</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>65.59166666666667</v>
       </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="n">
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="n">
         <v>15.2375</v>
       </c>
-      <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="n">
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="n">
         <v>31.5304347826087</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>19.33333333333333</v>
       </c>
-      <c r="S5" t="n">
+      <c r="T5" t="n">
         <v>11.22916666666667</v>
       </c>
-      <c r="T5" t="n">
+      <c r="U5" t="n">
         <v>38.375</v>
       </c>
-      <c r="U5" t="n">
+      <c r="V5" t="n">
         <v>31.28333333333333</v>
       </c>
-      <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="n">
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="n">
         <v>14.875</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AB5" t="n">
         <v>59.25</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AC5" t="n">
         <v>47.95833333333334</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AD5" t="n">
         <v>33.91666666666666</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AE5" t="n">
         <v>28.21666666666667</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AF5" t="n">
         <v>23.87916666666667</v>
       </c>
-      <c r="AF5" t="inlineStr"/>
-      <c r="AG5" t="n">
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="n">
         <v>3.416666666666667</v>
       </c>
-      <c r="AH5" t="n">
+      <c r="AI5" t="n">
         <v>21.1375</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AJ5" t="n">
         <v>18.47083333333333</v>
       </c>
-      <c r="AJ5" t="n">
+      <c r="AK5" t="n">
         <v>31.32916666666667</v>
       </c>
-      <c r="AK5" t="inlineStr"/>
-      <c r="AL5" t="n">
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="n">
         <v>24.01666666666667</v>
       </c>
-      <c r="AM5" t="inlineStr"/>
       <c r="AN5" t="inlineStr"/>
-      <c r="AO5" t="n">
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="n">
         <v>62.16666666666666</v>
       </c>
-      <c r="AP5" t="inlineStr"/>
-      <c r="AQ5" t="n">
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="n">
         <v>25.72916666666667</v>
       </c>
-      <c r="AR5" t="n">
+      <c r="AS5" t="n">
         <v>21.28333333333333</v>
       </c>
-      <c r="AS5" t="inlineStr"/>
-      <c r="AT5" t="n">
+      <c r="AT5" t="inlineStr"/>
+      <c r="AU5" t="n">
         <v>34.07916666666667</v>
       </c>
-      <c r="AU5" t="n">
+      <c r="AV5" t="n">
         <v>28.33333333333333</v>
       </c>
-      <c r="AV5" t="n">
+      <c r="AW5" t="n">
         <v>26.10416666666667</v>
       </c>
-      <c r="AW5" t="n">
+      <c r="AX5" t="n">
         <v>11.85833333333333</v>
       </c>
-      <c r="AX5" t="n">
+      <c r="AY5" t="n">
         <v>13.8375</v>
       </c>
-      <c r="AY5" t="inlineStr"/>
-      <c r="AZ5" t="n">
+      <c r="AZ5" t="inlineStr"/>
+      <c r="BA5" t="n">
         <v>11.7875</v>
       </c>
-      <c r="BA5" t="inlineStr"/>
-      <c r="BB5" t="n">
+      <c r="BB5" t="inlineStr"/>
+      <c r="BC5" t="n">
         <v>8.908333333333333</v>
       </c>
-      <c r="BC5" t="n">
+      <c r="BD5" t="n">
         <v>19.25416666666667</v>
       </c>
-      <c r="BD5" t="n">
+      <c r="BE5" t="n">
         <v>23.79166666666667</v>
       </c>
-      <c r="BE5" t="n">
+      <c r="BF5" t="n">
         <v>11.79166666666667</v>
       </c>
-      <c r="BF5" t="inlineStr"/>
-      <c r="BG5" t="n">
+      <c r="BG5" t="inlineStr"/>
+      <c r="BH5" t="n">
         <v>18.28571428571428</v>
       </c>
-      <c r="BH5" t="n">
-        <v>0.6440677966101694</v>
+      <c r="BI5" t="n">
+        <v>0.65</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="2" t="n">
+        <v>43026</v>
+      </c>
+      <c r="B6" t="n">
         <v>11.125</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>9.458333333333334</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>10.30416666666667</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>16.08333333333333</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>13.22083333333333</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>9.454545454545455</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>6.565217391304348</v>
       </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
         <v>14.81</v>
       </c>
-      <c r="J6" t="n">
+      <c r="K6" t="n">
         <v>8.529166666666667</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>15.5</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>20.07727272727273</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>9.826086956521738</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>5.916666666666667</v>
       </c>
-      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="n">
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="n">
         <v>21.97083333333333</v>
       </c>
-      <c r="R6" t="n">
+      <c r="S6" t="n">
         <v>8.666666666666666</v>
       </c>
-      <c r="S6" t="n">
+      <c r="T6" t="n">
         <v>8.491666666666667</v>
       </c>
-      <c r="T6" t="n">
+      <c r="U6" t="n">
         <v>5.983333333333333</v>
       </c>
-      <c r="U6" t="n">
+      <c r="V6" t="n">
         <v>13.31666666666667</v>
       </c>
-      <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
-      <c r="X6" t="n">
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="n">
         <v>12.66666666666667</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="Z6" t="n">
         <v>2.208333333333333</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="AA6" t="n">
         <v>4.125</v>
       </c>
-      <c r="AA6" t="n">
+      <c r="AB6" t="n">
         <v>14.25</v>
       </c>
-      <c r="AB6" t="n">
+      <c r="AC6" t="n">
         <v>5.958333333333333</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AD6" t="n">
         <v>12.75</v>
       </c>
-      <c r="AD6" t="n">
+      <c r="AE6" t="n">
         <v>10.64583333333333</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="AF6" t="n">
         <v>11.4125</v>
       </c>
-      <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="n">
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="n">
         <v>0</v>
       </c>
-      <c r="AH6" t="n">
+      <c r="AI6" t="n">
         <v>8.920833333333333</v>
       </c>
-      <c r="AI6" t="n">
+      <c r="AJ6" t="n">
         <v>6.1875</v>
       </c>
-      <c r="AJ6" t="n">
+      <c r="AK6" t="n">
         <v>15.86666666666667</v>
       </c>
-      <c r="AK6" t="inlineStr"/>
-      <c r="AL6" t="n">
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="n">
         <v>11.45833333333333</v>
       </c>
-      <c r="AM6" t="inlineStr"/>
       <c r="AN6" t="inlineStr"/>
-      <c r="AO6" t="n">
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="n">
         <v>8</v>
       </c>
-      <c r="AP6" t="inlineStr"/>
-      <c r="AQ6" t="n">
+      <c r="AQ6" t="inlineStr"/>
+      <c r="AR6" t="n">
         <v>17.29583333333333</v>
       </c>
-      <c r="AR6" t="n">
+      <c r="AS6" t="n">
         <v>9.191666666666666</v>
       </c>
-      <c r="AS6" t="n">
+      <c r="AT6" t="n">
         <v>13.33333333333333</v>
       </c>
-      <c r="AT6" t="n">
+      <c r="AU6" t="n">
         <v>14.77916666666667</v>
       </c>
-      <c r="AU6" t="n">
+      <c r="AV6" t="n">
         <v>5.238095238095238</v>
       </c>
-      <c r="AV6" t="n">
+      <c r="AW6" t="n">
         <v>8.491666666666667</v>
       </c>
-      <c r="AW6" t="n">
+      <c r="AX6" t="n">
         <v>6.6375</v>
       </c>
-      <c r="AX6" t="n">
+      <c r="AY6" t="n">
         <v>3.733333333333334</v>
       </c>
-      <c r="AY6" t="inlineStr"/>
-      <c r="AZ6" t="n">
+      <c r="AZ6" t="inlineStr"/>
+      <c r="BA6" t="n">
         <v>17.42916666666667</v>
       </c>
-      <c r="BA6" t="inlineStr"/>
-      <c r="BB6" t="n">
+      <c r="BB6" t="inlineStr"/>
+      <c r="BC6" t="n">
         <v>15.65833333333333</v>
       </c>
-      <c r="BC6" t="n">
+      <c r="BD6" t="n">
         <v>24.78333333333333</v>
       </c>
-      <c r="BD6" t="n">
+      <c r="BE6" t="n">
         <v>9.625</v>
       </c>
-      <c r="BE6" t="n">
+      <c r="BF6" t="n">
         <v>5.666666666666667</v>
       </c>
-      <c r="BF6" t="n">
+      <c r="BG6" t="n">
         <v>21.66666666666667</v>
       </c>
-      <c r="BG6" t="n">
+      <c r="BH6" t="n">
         <v>10.91666666666667</v>
       </c>
-      <c r="BH6" t="n">
-        <v>0.7966101694915254</v>
+      <c r="BI6" t="n">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>